<commit_message>
Fix quote and split of values
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_bexsta_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_bexsta_by_metamake.xlsx
@@ -44,7 +44,7 @@
     <t xml:space="preserve">LANGUAGES</t>
   </si>
   <si>
-    <t xml:space="preserve">en,da,kl</t>
+    <t xml:space="preserve">en","da","kl</t>
   </si>
   <si>
     <t xml:space="preserve">CREATION-DATE</t>
@@ -1617,13 +1617,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
         <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
         <v>134</v>
@@ -1631,13 +1631,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
         <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
@@ -1645,13 +1645,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>133</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
         <v>136</v>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
         <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>138</v>
@@ -1673,13 +1673,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
         <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
         <v>139</v>
@@ -1687,13 +1687,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
         <v>140</v>
@@ -1701,13 +1701,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
         <v>141</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
         <v>142</v>
@@ -1715,13 +1715,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
         <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
         <v>143</v>
@@ -1729,13 +1729,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
         <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
         <v>144</v>
@@ -1743,13 +1743,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
         <v>146</v>
@@ -1757,13 +1757,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
         <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
         <v>147</v>
@@ -1771,13 +1771,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
         <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
         <v>148</v>
@@ -1785,13 +1785,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
         <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
         <v>150</v>
@@ -1799,13 +1799,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
         <v>149</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" t="s">
         <v>151</v>
@@ -1813,13 +1813,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
         <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
         <v>152</v>
@@ -1827,13 +1827,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
         <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
         <v>153</v>
@@ -1841,13 +1841,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
         <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
         <v>154</v>
@@ -1855,13 +1855,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
         <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
         <v>155</v>
@@ -1869,13 +1869,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
         <v>137</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
         <v>156</v>
@@ -1883,13 +1883,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
         <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
         <v>157</v>
@@ -1897,13 +1897,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
         <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
         <v>158</v>
@@ -1911,13 +1911,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
         <v>141</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D23" t="s">
         <v>159</v>
@@ -1925,13 +1925,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
         <v>141</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D24" t="s">
         <v>160</v>
@@ -1939,13 +1939,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
         <v>141</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D25" t="s">
         <v>161</v>
@@ -1953,13 +1953,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
         <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
         <v>162</v>
@@ -1967,13 +1967,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
         <v>145</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D27" t="s">
         <v>163</v>
@@ -1981,13 +1981,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
         <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D28" t="s">
         <v>164</v>
@@ -1995,13 +1995,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
         <v>149</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
         <v>165</v>
@@ -2009,13 +2009,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
         <v>149</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30" t="s">
         <v>166</v>
@@ -2023,13 +2023,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B31" t="s">
         <v>149</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D31" t="s">
         <v>167</v>
@@ -2037,13 +2037,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" t="s">
         <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D32" t="s">
         <v>168</v>
@@ -2051,13 +2051,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" t="s">
         <v>133</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
         <v>169</v>
@@ -2065,13 +2065,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B34" t="s">
         <v>133</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D34" t="s">
         <v>170</v>
@@ -2079,13 +2079,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s">
         <v>137</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D35" t="s">
         <v>171</v>
@@ -2093,13 +2093,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B36" t="s">
         <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
         <v>172</v>
@@ -2107,13 +2107,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
         <v>137</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D37" t="s">
         <v>173</v>
@@ -2121,13 +2121,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
         <v>141</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
         <v>174</v>
@@ -2135,13 +2135,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
         <v>141</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
         <v>175</v>
@@ -2149,13 +2149,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" t="s">
         <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D40" t="s">
         <v>176</v>
@@ -2163,13 +2163,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B41" t="s">
         <v>145</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
         <v>177</v>
@@ -2177,13 +2177,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
         <v>145</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42" t="s">
         <v>178</v>
@@ -2191,13 +2191,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" t="s">
         <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D43" t="s">
         <v>179</v>
@@ -2205,13 +2205,13 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B44" t="s">
         <v>149</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D44" t="s">
         <v>180</v>
@@ -2219,13 +2219,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
         <v>149</v>
       </c>
       <c r="C45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
         <v>181</v>
@@ -2233,13 +2233,13 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
         <v>149</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D46" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Add argument to let metamake save data cube in rds file
Close #108
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_bexsta_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_bexsta_by_metamake.xlsx
@@ -9,13 +9,12 @@
     <sheet name="Table" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Variables" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Codelists" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t xml:space="preserve">keyword</t>
   </si>
@@ -417,156 +416,6 @@
   </si>
   <si>
     <t xml:space="preserve">Kalaallit Nunaata avataani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55877</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29489</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26388</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29553</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26439</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29551</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26530</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56421</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29749</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26672</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29803</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26759</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24392</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50251</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24434</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24541</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50388</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24578</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5706</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3710</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1996</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5741</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3736</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5891</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3813</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2181</t>
   </si>
 </sst>
 </file>
@@ -659,19 +508,6 @@
     <tableColumn id="5" name="da_code_label"/>
     <tableColumn id="6" name="kl_code_label"/>
     <tableColumn id="7" name="precision"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D46" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D46"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="place of birth"/>
-    <tableColumn id="2" name="time"/>
-    <tableColumn id="3" name="gender"/>
-    <tableColumn id="4" name=".figures"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1685,671 +1521,4 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="14.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="4.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="6.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="8.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" t="s">
-        <v>138</v>
-      </c>
-      <c r="C20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" t="s">
-        <v>138</v>
-      </c>
-      <c r="C21" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C22" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C23" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C25" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C26" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" t="s">
-        <v>122</v>
-      </c>
-      <c r="D28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C29" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>130</v>
-      </c>
-      <c r="B32" t="s">
-        <v>134</v>
-      </c>
-      <c r="C32" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B34" t="s">
-        <v>134</v>
-      </c>
-      <c r="C34" t="s">
-        <v>122</v>
-      </c>
-      <c r="D34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>130</v>
-      </c>
-      <c r="B35" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>130</v>
-      </c>
-      <c r="B36" t="s">
-        <v>138</v>
-      </c>
-      <c r="C36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>130</v>
-      </c>
-      <c r="B37" t="s">
-        <v>138</v>
-      </c>
-      <c r="C37" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>130</v>
-      </c>
-      <c r="B38" t="s">
-        <v>142</v>
-      </c>
-      <c r="C38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>130</v>
-      </c>
-      <c r="B39" t="s">
-        <v>142</v>
-      </c>
-      <c r="C39" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>130</v>
-      </c>
-      <c r="B40" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>130</v>
-      </c>
-      <c r="B41" t="s">
-        <v>146</v>
-      </c>
-      <c r="C41" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" t="s">
-        <v>146</v>
-      </c>
-      <c r="C42" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" t="s">
-        <v>146</v>
-      </c>
-      <c r="C43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" t="s">
-        <v>117</v>
-      </c>
-      <c r="D44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>130</v>
-      </c>
-      <c r="B45" t="s">
-        <v>150</v>
-      </c>
-      <c r="C45" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>130</v>
-      </c>
-      <c r="B46" t="s">
-        <v>150</v>
-      </c>
-      <c r="C46" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId6"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add test for quotes around YES/NO
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_bexsta_by_metamake.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_bexsta_by_metamake.xlsx
@@ -9,12 +9,13 @@
     <sheet name="Table" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Variables" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Codelists" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t xml:space="preserve">keyword</t>
   </si>
@@ -419,6 +420,156 @@
   </si>
   <si>
     <t xml:space="preserve">Kalaallit Nunaata avataani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29553</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24541</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5891</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2181</t>
   </si>
 </sst>
 </file>
@@ -511,6 +662,19 @@
     <tableColumn id="5" name="da_code_label"/>
     <tableColumn id="6" name="kl_code_label"/>
     <tableColumn id="7" name="precision"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D46" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D46"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="place of birth"/>
+    <tableColumn id="2" name="time"/>
+    <tableColumn id="3" name="gender"/>
+    <tableColumn id="4" name="figures_"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1524,4 +1688,671 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="14.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="4.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="6.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="8.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>